<commit_message>
doc updates for 3d printed parts and new modular PCB
</commit_message>
<xml_diff>
--- a/doc_src/source/BOMs/hardware bom.xlsx
+++ b/doc_src/source/BOMs/hardware bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/Syringe/Documentation Source/source/BOMs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/Syringe/doc_src/source/BOMs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAD3BAA-E360-AD4E-A361-6265B83EB9BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F070B6-AB96-2848-89F7-BA86A9BD0B56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
   <si>
     <t>link</t>
   </si>
@@ -69,51 +69,18 @@
     <t>McMaster-Carr</t>
   </si>
   <si>
-    <t>Grommet</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#9600k54</t>
-  </si>
-  <si>
-    <t>9600k54</t>
-  </si>
-  <si>
-    <t>92005A220</t>
-  </si>
-  <si>
     <t>94510A240</t>
   </si>
   <si>
-    <t>96887A329</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#96887A329</t>
-  </si>
-  <si>
-    <t>M4  square nut</t>
-  </si>
-  <si>
     <t>https://www.mcmaster.com/#94510A240</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>https://www.servocity.com/lead-screws#371=448</t>
-  </si>
-  <si>
-    <t>ServoCity</t>
-  </si>
-  <si>
-    <t>https://www.servocity.com/8mm-stainless-steel-precision-shafting#371=460</t>
-  </si>
-  <si>
     <t>200 x  8 mm shaft</t>
   </si>
   <si>
-    <t>https://www.servocity.com/8mm-4-start-hub</t>
-  </si>
-  <si>
     <t>8mm lead screw nut</t>
   </si>
   <si>
@@ -123,9 +90,6 @@
     <t>Amazon</t>
   </si>
   <si>
-    <t>https://www.mcmaster.com/#92005A226</t>
-  </si>
-  <si>
     <t>https://www.mcmaster.com/#92000A120</t>
   </si>
   <si>
@@ -168,9 +132,6 @@
     <t>Qty to order</t>
   </si>
   <si>
-    <t>12" x 12" x 1/4" Acrylic</t>
-  </si>
-  <si>
     <t>for 5</t>
   </si>
   <si>
@@ -195,30 +156,12 @@
     <t>.25" clear acylic</t>
   </si>
   <si>
-    <t>7804K147</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#7804K147</t>
-  </si>
-  <si>
     <t>92005A130</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/#92005A130</t>
   </si>
   <si>
-    <t>92005A132</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#92005A132</t>
-  </si>
-  <si>
-    <t>4615T37</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#4615T37</t>
-  </si>
-  <si>
     <t>Spring</t>
   </si>
   <si>
@@ -228,9 +171,6 @@
     <t>9657K267</t>
   </si>
   <si>
-    <t>M4 x 16mm machine screw</t>
-  </si>
-  <si>
     <t>M3 x 25mm machine screw</t>
   </si>
   <si>
@@ -243,33 +183,12 @@
     <t>Nema 17 bipolar 60Ncm 200steps</t>
   </si>
   <si>
-    <t>M3 x 30mm machine screw</t>
-  </si>
-  <si>
-    <t>Flanged ball bearing</t>
-  </si>
-  <si>
-    <t>Flanged LMF8UU slide bearing</t>
-  </si>
-  <si>
-    <t>B00NQ2H8YUF17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">350 x 8mm lead screw </t>
-  </si>
-  <si>
-    <t>3501-0804-0350</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/Befenybay-Coupling-Diameter-Coupler-Aluminum/dp/B07Q5Q3DCB/ref=sr_1_1?keywords=B07Q5Q3DCB&amp;qid=1565137893&amp;s=gateway&amp;sr=8-1</t>
   </si>
   <si>
     <t>B07Q5Q3DCB</t>
   </si>
   <si>
-    <t>https://www.amazon.com/s?k=LMF8UU&amp;ref=nb_sb_noss_2</t>
-  </si>
-  <si>
     <t>Limit Switch</t>
   </si>
   <si>
@@ -279,25 +198,75 @@
     <t>277-2296-ND</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
     <t>DIN clip</t>
+  </si>
+  <si>
+    <t>https://www.gobilda.com/2100-series-stainless-steel-round-shaft-8mm-diameter-200mm-length/</t>
+  </si>
+  <si>
+    <t>https://www.gobilda.com/3505-series-lead-screw-pattern-nut-8mm-lead-4-start-32mm-od-16mm-length/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250 x 8mm lead screw </t>
+  </si>
+  <si>
+    <t>https://www.gobilda.com/3501-series-lead-screw-8mm-lead-4-start-250mm-length/</t>
+  </si>
+  <si>
+    <t>goBILDA</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>97259A101</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/97259A101/</t>
+  </si>
+  <si>
+    <t>M3 x 16mm machine screw</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92005A126/</t>
+  </si>
+  <si>
+    <t>92005A126</t>
+  </si>
+  <si>
+    <t>M3 Thin square nut</t>
+  </si>
+  <si>
+    <t>Linear ball bearing</t>
+  </si>
+  <si>
+    <t>https://www.gobilda.com/1612-series-linear-ball-bearing-8mm-id-x-15mm-od-45mm-length-2-pack/</t>
+  </si>
+  <si>
+    <t>1612-0815-0045</t>
+  </si>
+  <si>
+    <t>3505-0804-3216</t>
+  </si>
+  <si>
+    <t>3501-0804-0250</t>
+  </si>
+  <si>
+    <t>2100-0008-0200</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#\ &quot;Assemblies&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -367,6 +336,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -374,7 +380,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -392,9 +398,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -407,17 +410,38 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -541,7 +565,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>BOM!$L$4:$L$14</c:f>
+              <c:f>BOM!$AB$4:$AB$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -580,39 +604,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>BOM!$N$4:$N$14</c:f>
+              <c:f>BOM!$AD$4:$AD$14</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>179.60000000000002</c:v>
+                  <c:v>106.07</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>135.40999999999997</c:v>
+                  <c:v>76.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>127.21000000000002</c:v>
+                  <c:v>71.930000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120.84</c:v>
+                  <c:v>68.167500000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>125.154</c:v>
+                  <c:v>67.204000000000008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>117.39400000000001</c:v>
+                  <c:v>63.731666666666662</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>114.23166666666668</c:v>
+                  <c:v>65.178571428571431</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>112.82874999999999</c:v>
+                  <c:v>62.827500000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>111.80444444444443</c:v>
+                  <c:v>62.885555555555555</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>110.797</c:v>
+                  <c:v>62.285000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1006,7 +1030,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>BOM!$L$4:$L$13</c:f>
+              <c:f>BOM!$AB$4:$AB$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1045,39 +1069,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>BOM!$N$4:$N$13</c:f>
+              <c:f>BOM!$AD$4:$AD$13</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>179.60000000000002</c:v>
+                  <c:v>106.07</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>135.40999999999997</c:v>
+                  <c:v>76.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>127.21000000000002</c:v>
+                  <c:v>71.930000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120.84</c:v>
+                  <c:v>68.167500000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>125.154</c:v>
+                  <c:v>67.204000000000008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>117.39400000000001</c:v>
+                  <c:v>63.731666666666662</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>114.23166666666668</c:v>
+                  <c:v>65.178571428571431</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>112.82874999999999</c:v>
+                  <c:v>62.827500000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>111.80444444444443</c:v>
+                  <c:v>62.885555555555555</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>110.797</c:v>
+                  <c:v>62.285000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2392,13 +2416,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
@@ -2430,16 +2454,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2730,1076 +2754,1921 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA20"/>
+  <dimension ref="A1:AQ17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="165.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="12" width="13" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="22" width="10.83203125" style="1"/>
-    <col min="23" max="23" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.6640625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.83203125" style="1"/>
+    <col min="28" max="28" width="13" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="38" width="10.83203125" style="1"/>
+    <col min="39" max="39" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:43" s="15" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="I1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="20">
+        <v>1</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="20">
+        <v>2</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="20">
+        <v>4</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="20">
+        <v>6</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="20">
+        <v>8</v>
+      </c>
+      <c r="X1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="20">
+        <v>10</v>
+      </c>
+      <c r="AB1" s="21">
+        <f>SUM(K2:K16)</f>
+        <v>111.22</v>
+      </c>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
     </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="3">
-        <v>1</v>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:C12" si="0">CONCATENATE("`",E2," &lt;",F2,"&gt;`_")</f>
-        <v>`4615T37 &lt;https://www.mcmaster.com/#4615T37&gt;`_</v>
+        <f t="shared" ref="C2:C16" si="0">CONCATENATE("`",E2," &lt;",F2,"&gt;`_")</f>
+        <v>`92005A130 &lt;https://www.mcmaster.com/#92005A130&gt;`_</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>59</v>
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="G2" s="6">
-        <v>31.84</v>
+        <v>3.36</v>
       </c>
       <c r="H2" s="1">
-        <v>1</v>
-      </c>
-      <c r="I2" s="7">
-        <f>A2*BOM!$L$2</f>
-        <v>10</v>
-      </c>
-      <c r="J2" s="7">
-        <f t="shared" ref="J2:J4" si="1">ROUNDUP(I2/H2,0)</f>
-        <v>10</v>
-      </c>
-      <c r="K2" s="1">
-        <f>J2*G2/BOM!$L$2</f>
-        <v>31.839999999999996</v>
-      </c>
-      <c r="L2" s="12">
-        <v>10</v>
-      </c>
-      <c r="M2" s="11">
-        <f>SUMPRODUCT(BOM!J2:J20,BOM!G2:G20)</f>
-        <v>1032.0099999999998</v>
-      </c>
-      <c r="N2" s="11">
-        <f>M2/L2</f>
-        <v>103.20099999999998</v>
-      </c>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
+        <v>100</v>
+      </c>
+      <c r="I2" s="17">
+        <f xml:space="preserve"> $A2*K$1</f>
+        <v>4</v>
+      </c>
+      <c r="J2" s="17">
+        <f>ROUNDUP(I2/$H2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
+        <f>J2*$G2/K$1</f>
+        <v>3.36</v>
+      </c>
+      <c r="L2" s="17">
+        <f xml:space="preserve"> $A2*N$1</f>
+        <v>8</v>
+      </c>
+      <c r="M2" s="17">
+        <f>ROUNDUP(L2/$H2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N2" s="6">
+        <f>M2*$G2/N$1</f>
+        <v>1.68</v>
+      </c>
+      <c r="O2" s="17">
+        <f xml:space="preserve"> $A2*Q$1</f>
+        <v>16</v>
+      </c>
+      <c r="P2" s="17">
+        <f>ROUNDUP(O2/$H2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q2" s="6">
+        <f>P2*$G2/Q$1</f>
+        <v>0.84</v>
+      </c>
+      <c r="R2" s="17">
+        <f xml:space="preserve"> $A2*T$1</f>
+        <v>24</v>
+      </c>
+      <c r="S2" s="17">
+        <f>ROUNDUP(R2/$H2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="T2" s="6">
+        <f>S2*$G2/T$1</f>
+        <v>0.55999999999999994</v>
+      </c>
+      <c r="U2" s="17">
+        <f xml:space="preserve"> $A2*W$1</f>
+        <v>32</v>
+      </c>
+      <c r="V2" s="17">
+        <f>ROUNDUP(U2/$H2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="W2" s="6">
+        <f>V2*$G2/W$1</f>
+        <v>0.42</v>
+      </c>
+      <c r="X2" s="17">
+        <f xml:space="preserve"> $A2*Z$1</f>
+        <v>40</v>
+      </c>
+      <c r="Y2" s="17">
+        <f>ROUNDUP(X2/$H2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z2" s="6">
+        <f>Y2*$G2/Z$1</f>
+        <v>0.33599999999999997</v>
+      </c>
+      <c r="AC2" s="10">
+        <f>SUMPRODUCT(BOM!J2:J16,BOM!G2:G16)</f>
+        <v>111.22</v>
+      </c>
+      <c r="AD2" s="10">
+        <f>AC2/K1</f>
+        <v>111.22</v>
+      </c>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
     </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="3">
-        <v>2</v>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>`9600k54 &lt;https://www.mcmaster.com/#9600k54&gt;`_</v>
+        <v>`92005A126 &lt;https://www.mcmaster.com/92005A126/&gt;`_</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="6">
-        <v>10.52</v>
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3.9</v>
       </c>
       <c r="H3" s="1">
-        <v>50</v>
-      </c>
-      <c r="I3" s="7">
-        <f>A3*BOM!$L$2</f>
-        <v>20</v>
-      </c>
-      <c r="J3" s="7">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
-        <f>J3*G3/BOM!$L$2</f>
-        <v>1.052</v>
-      </c>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
+        <v>100</v>
+      </c>
+      <c r="I3" s="17">
+        <f t="shared" ref="I3:I16" si="1" xml:space="preserve"> $A3*K$1</f>
+        <v>4</v>
+      </c>
+      <c r="J3" s="17">
+        <f t="shared" ref="J3:J16" si="2">ROUNDUP(I3/$H3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="6">
+        <f t="shared" ref="K3:K16" si="3">J3*$G3/K$1</f>
+        <v>3.9</v>
+      </c>
+      <c r="L3" s="17">
+        <f t="shared" ref="L3:L16" si="4" xml:space="preserve"> $A3*N$1</f>
+        <v>8</v>
+      </c>
+      <c r="M3" s="17">
+        <f t="shared" ref="M3:M16" si="5">ROUNDUP(L3/$H3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="6">
+        <f t="shared" ref="N3:N16" si="6">M3*$G3/N$1</f>
+        <v>1.95</v>
+      </c>
+      <c r="O3" s="17">
+        <f t="shared" ref="O3:O16" si="7" xml:space="preserve"> $A3*Q$1</f>
+        <v>16</v>
+      </c>
+      <c r="P3" s="17">
+        <f t="shared" ref="P3:P16" si="8">ROUNDUP(O3/$H3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6">
+        <f t="shared" ref="Q3:Q16" si="9">P3*$G3/Q$1</f>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="R3" s="17">
+        <f t="shared" ref="R3:R16" si="10" xml:space="preserve"> $A3*T$1</f>
+        <v>24</v>
+      </c>
+      <c r="S3" s="17">
+        <f t="shared" ref="S3:S16" si="11">ROUNDUP(R3/$H3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="T3" s="6">
+        <f t="shared" ref="T3:T16" si="12">S3*$G3/T$1</f>
+        <v>0.65</v>
+      </c>
+      <c r="U3" s="17">
+        <f t="shared" ref="U3:U16" si="13" xml:space="preserve"> $A3*W$1</f>
+        <v>32</v>
+      </c>
+      <c r="V3" s="17">
+        <f t="shared" ref="V3:V16" si="14">ROUNDUP(U3/$H3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="W3" s="6">
+        <f t="shared" ref="W3:W16" si="15">V3*$G3/W$1</f>
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="X3" s="17">
+        <f t="shared" ref="X3:X16" si="16" xml:space="preserve"> $A3*Z$1</f>
+        <v>40</v>
+      </c>
+      <c r="Y3" s="17">
+        <f t="shared" ref="Y3:Y16" si="17">ROUNDUP(X3/$H3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z3" s="6">
+        <f t="shared" ref="Z3:Z16" si="18">Y3*$G3/Z$1</f>
+        <v>0.39</v>
+      </c>
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
+      <c r="AK3"/>
+      <c r="AL3"/>
     </row>
-    <row r="4" spans="1:27">
-      <c r="A4" s="3">
-        <v>1</v>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>`7804K147 &lt;https://www.mcmaster.com/#7804K147&gt;`_</v>
+        <v>`92000A120 &lt;https://www.mcmaster.com/#92000A120&gt;`_</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="G4" s="6">
-        <v>7.97</v>
+        <v>4.7</v>
       </c>
       <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="7">
-        <f>A4*BOM!$L$2</f>
-        <v>10</v>
-      </c>
-      <c r="J4" s="7">
+        <v>100</v>
+      </c>
+      <c r="I4" s="17">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="K4" s="1">
-        <f>J4*G4/BOM!$L$2</f>
-        <v>7.9700000000000006</v>
-      </c>
-      <c r="L4" s="13">
-        <v>1</v>
-      </c>
-      <c r="M4" s="11">
-        <v>179.60000000000002</v>
-      </c>
-      <c r="N4" s="11">
-        <v>179.60000000000002</v>
-      </c>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
+      <c r="J4" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K4" s="6">
+        <f t="shared" si="3"/>
+        <v>4.7</v>
+      </c>
+      <c r="L4" s="17">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="M4" s="17">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N4" s="6">
+        <f t="shared" si="6"/>
+        <v>2.35</v>
+      </c>
+      <c r="O4" s="17">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="P4" s="17">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="6">
+        <f t="shared" si="9"/>
+        <v>1.175</v>
+      </c>
+      <c r="R4" s="17">
+        <f t="shared" si="10"/>
+        <v>60</v>
+      </c>
+      <c r="S4" s="17">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="T4" s="6">
+        <f t="shared" si="12"/>
+        <v>0.78333333333333333</v>
+      </c>
+      <c r="U4" s="17">
+        <f t="shared" si="13"/>
+        <v>80</v>
+      </c>
+      <c r="V4" s="17">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="W4" s="6">
+        <f t="shared" si="15"/>
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="X4" s="17">
+        <f t="shared" si="16"/>
+        <v>100</v>
+      </c>
+      <c r="Y4" s="17">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="Z4" s="6">
+        <f t="shared" si="18"/>
+        <v>0.47000000000000003</v>
+      </c>
+      <c r="AB4" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="10">
+        <v>106.07</v>
+      </c>
+      <c r="AD4" s="10">
+        <v>106.07</v>
+      </c>
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AG4"/>
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AJ4"/>
+      <c r="AK4"/>
+      <c r="AL4"/>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>`92005A220 &lt;https://www.mcmaster.com/#92005A226&gt;`_</v>
+        <v>`97259A101 &lt;https://www.mcmaster.com/97259A101/&gt;`_</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
       </c>
       <c r="G5" s="6">
-        <v>4.4000000000000004</v>
+        <v>8</v>
       </c>
       <c r="H5" s="1">
         <v>100</v>
       </c>
-      <c r="I5" s="7">
-        <f>A5*BOM!$L$2</f>
+      <c r="I5" s="17">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J5" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="6">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="L5" s="17">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="M5" s="17">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N5" s="6">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="O5" s="17">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="P5" s="17">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="6">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="R5" s="17">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="S5" s="17">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="T5" s="6">
+        <f t="shared" si="12"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="U5" s="17">
+        <f t="shared" si="13"/>
+        <v>32</v>
+      </c>
+      <c r="V5" s="17">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="W5" s="6">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="X5" s="17">
+        <f t="shared" si="16"/>
         <v>40</v>
       </c>
-      <c r="J5" s="7">
-        <f t="shared" ref="J5:J20" si="2">ROUNDUP(I5/H5,0)</f>
-        <v>1</v>
-      </c>
-      <c r="K5" s="1">
-        <f>J5*G5/BOM!$L$2</f>
-        <v>0.44000000000000006</v>
-      </c>
-      <c r="L5" s="13">
+      <c r="Y5" s="17">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="Z5" s="6">
+        <f t="shared" si="18"/>
+        <v>0.8</v>
+      </c>
+      <c r="AB5" s="11">
         <v>2</v>
       </c>
-      <c r="M5" s="11">
-        <v>270.81999999999994</v>
-      </c>
-      <c r="N5" s="11">
-        <v>135.40999999999997</v>
-      </c>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5"/>
+      <c r="AC5" s="10">
+        <v>152.44</v>
+      </c>
+      <c r="AD5" s="10">
+        <v>76.22</v>
+      </c>
+      <c r="AE5"/>
+      <c r="AF5"/>
+      <c r="AG5"/>
+      <c r="AH5"/>
+      <c r="AI5"/>
+      <c r="AJ5"/>
+      <c r="AK5"/>
+      <c r="AL5"/>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>`96887A329 &lt;https://www.mcmaster.com/#96887A329&gt;`_</v>
+        <v>`94510A240 &lt;https://www.mcmaster.com/#94510A240&gt;`_</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G6" s="6">
-        <v>10</v>
+        <v>7.2</v>
       </c>
       <c r="H6" s="1">
-        <v>100</v>
-      </c>
-      <c r="I6" s="7">
-        <f>A6*BOM!$L$2</f>
-        <v>40</v>
-      </c>
-      <c r="J6" s="7">
+        <v>50</v>
+      </c>
+      <c r="I6" s="17">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J6" s="17">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K6" s="1">
-        <f>J6*G6/BOM!$L$2</f>
-        <v>1</v>
-      </c>
-      <c r="L6" s="13">
+      <c r="K6" s="6">
+        <f t="shared" si="3"/>
+        <v>7.2</v>
+      </c>
+      <c r="L6" s="17">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="M6" s="17">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N6" s="6">
+        <f t="shared" si="6"/>
+        <v>3.6</v>
+      </c>
+      <c r="O6" s="17">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="P6" s="17">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="Q6" s="6">
+        <f t="shared" si="9"/>
+        <v>1.8</v>
+      </c>
+      <c r="R6" s="17">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="S6" s="17">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="T6" s="6">
+        <f t="shared" si="12"/>
+        <v>1.2</v>
+      </c>
+      <c r="U6" s="17">
+        <f t="shared" si="13"/>
+        <v>24</v>
+      </c>
+      <c r="V6" s="17">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="W6" s="6">
+        <f t="shared" si="15"/>
+        <v>0.9</v>
+      </c>
+      <c r="X6" s="17">
+        <f t="shared" si="16"/>
+        <v>30</v>
+      </c>
+      <c r="Y6" s="17">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="Z6" s="6">
+        <f t="shared" si="18"/>
+        <v>0.72</v>
+      </c>
+      <c r="AB6" s="11">
         <v>3</v>
       </c>
-      <c r="M6" s="11">
-        <v>381.63000000000005</v>
-      </c>
-      <c r="N6" s="11">
-        <v>127.21000000000002</v>
-      </c>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
+      <c r="AC6" s="10">
+        <v>215.79000000000002</v>
+      </c>
+      <c r="AD6" s="10">
+        <v>71.930000000000007</v>
+      </c>
+      <c r="AE6"/>
+      <c r="AF6"/>
+      <c r="AG6"/>
+      <c r="AH6"/>
+      <c r="AI6"/>
+      <c r="AJ6"/>
+      <c r="AK6"/>
+      <c r="AL6"/>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>`92005A130 &lt;https://www.mcmaster.com/#92005A130&gt;`_</v>
+        <v>`9657K267 &lt;https://www.mcmaster.com/#9657K267&gt;`_</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G7" s="6">
-        <v>3.36</v>
+        <v>10.51</v>
       </c>
       <c r="H7" s="1">
-        <v>100</v>
-      </c>
-      <c r="I7" s="7">
-        <f>A7*BOM!$L$2</f>
+        <v>12</v>
+      </c>
+      <c r="I7" s="17">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J7" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" si="3"/>
+        <v>10.51</v>
+      </c>
+      <c r="L7" s="17">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="M7" s="17">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N7" s="6">
+        <f t="shared" si="6"/>
+        <v>5.2549999999999999</v>
+      </c>
+      <c r="O7" s="17">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="P7" s="17">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="Q7" s="6">
+        <f t="shared" si="9"/>
+        <v>5.2549999999999999</v>
+      </c>
+      <c r="R7" s="17">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="S7" s="17">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="T7" s="6">
+        <f t="shared" si="12"/>
+        <v>3.5033333333333334</v>
+      </c>
+      <c r="U7" s="17">
+        <f t="shared" si="13"/>
+        <v>32</v>
+      </c>
+      <c r="V7" s="17">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="W7" s="6">
+        <f t="shared" si="15"/>
+        <v>3.9412500000000001</v>
+      </c>
+      <c r="X7" s="17">
+        <f t="shared" si="16"/>
         <v>40</v>
       </c>
-      <c r="J7" s="7">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K7" s="1">
-        <f>J7*G7/BOM!$L$2</f>
-        <v>0.33599999999999997</v>
-      </c>
-      <c r="L7" s="13">
+      <c r="Y7" s="17">
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
-      <c r="M7" s="11">
-        <v>483.36</v>
-      </c>
-      <c r="N7" s="11">
-        <v>120.84</v>
-      </c>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
+      <c r="Z7" s="6">
+        <f t="shared" si="18"/>
+        <v>4.2039999999999997</v>
+      </c>
+      <c r="AB7" s="11">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="10">
+        <v>272.67</v>
+      </c>
+      <c r="AD7" s="10">
+        <v>68.167500000000004</v>
+      </c>
+      <c r="AE7"/>
+      <c r="AF7"/>
+      <c r="AG7"/>
+      <c r="AH7"/>
+      <c r="AI7"/>
+      <c r="AJ7"/>
+      <c r="AK7"/>
+      <c r="AL7"/>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>`92005A132 &lt;https://www.mcmaster.com/#92005A132&gt;`_</v>
+        <v>`6479K78 &lt;https://www.mcmaster.com/#6479K78&gt;`_</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="6">
+        <v>5.33</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" si="3"/>
+        <v>5.33</v>
+      </c>
+      <c r="L8" s="17">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M8" s="17">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N8" s="6">
+        <f t="shared" si="6"/>
+        <v>5.33</v>
+      </c>
+      <c r="O8" s="17">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="P8" s="17">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="Q8" s="6">
+        <f t="shared" si="9"/>
+        <v>5.33</v>
+      </c>
+      <c r="R8" s="17">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="S8" s="17">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="T8" s="6">
+        <f t="shared" si="12"/>
+        <v>5.33</v>
+      </c>
+      <c r="U8" s="17">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="V8" s="17">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="W8" s="6">
+        <f t="shared" si="15"/>
+        <v>5.33</v>
+      </c>
+      <c r="X8" s="17">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="Y8" s="17">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="Z8" s="6">
+        <f t="shared" si="18"/>
+        <v>5.33</v>
+      </c>
+      <c r="AB8" s="11">
+        <v>5</v>
+      </c>
+      <c r="AC8" s="10">
+        <v>336.02000000000004</v>
+      </c>
+      <c r="AD8" s="10">
+        <v>67.204000000000008</v>
+      </c>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
+      <c r="AK8"/>
+      <c r="AL8"/>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="6">
-        <v>3.88</v>
-      </c>
-      <c r="H8" s="1">
-        <v>100</v>
-      </c>
-      <c r="I8" s="7">
-        <f>A8*BOM!$L$2</f>
-        <v>40</v>
-      </c>
-      <c r="J8" s="7">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K8" s="1">
-        <f>J8*G8/BOM!$L$2</f>
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="L8" s="13">
-        <v>5</v>
-      </c>
-      <c r="M8" s="11">
-        <v>625.77</v>
-      </c>
-      <c r="N8" s="11">
-        <f t="shared" ref="N8" si="3">M8/L8</f>
-        <v>125.154</v>
-      </c>
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
-      <c r="R8"/>
-      <c r="S8"/>
-      <c r="T8"/>
-      <c r="U8"/>
-      <c r="V8"/>
-    </row>
-    <row r="9" spans="1:27">
-      <c r="A9" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>`92000A120 &lt;https://www.mcmaster.com/#92000A120&gt;`_</v>
+        <v>`3501-0804-0250 &lt;https://www.gobilda.com/3501-series-lead-screw-8mm-lead-4-start-250mm-length/&gt;`_</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>29</v>
+        <v>71</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
       </c>
       <c r="G9" s="6">
-        <v>4.7</v>
+        <v>6.99</v>
       </c>
       <c r="H9" s="1">
-        <v>100</v>
-      </c>
-      <c r="I9" s="7">
-        <f>A9*BOM!$L$2</f>
-        <v>220</v>
-      </c>
-      <c r="J9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="17">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="K9" s="1">
-        <f>J9*G9/BOM!$L$2</f>
-        <v>1.4100000000000001</v>
-      </c>
-      <c r="L9" s="13">
+        <v>1</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="3"/>
+        <v>6.99</v>
+      </c>
+      <c r="L9" s="17">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M9" s="17">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N9" s="6">
+        <f t="shared" si="6"/>
+        <v>6.99</v>
+      </c>
+      <c r="O9" s="17">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="P9" s="17">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="Q9" s="6">
+        <f t="shared" si="9"/>
+        <v>6.99</v>
+      </c>
+      <c r="R9" s="17">
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
-      <c r="M9" s="11">
-        <v>586.97</v>
-      </c>
-      <c r="N9" s="11">
-        <v>117.39400000000001</v>
-      </c>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-      <c r="R9"/>
-      <c r="S9"/>
-      <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
+      <c r="S9" s="17">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="T9" s="6">
+        <f t="shared" si="12"/>
+        <v>6.9899999999999993</v>
+      </c>
+      <c r="U9" s="17">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="V9" s="17">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="W9" s="6">
+        <f t="shared" si="15"/>
+        <v>6.99</v>
+      </c>
+      <c r="X9" s="17">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="Y9" s="17">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="Z9" s="6">
+        <f t="shared" si="18"/>
+        <v>6.99</v>
+      </c>
+      <c r="AB9" s="11">
+        <v>6</v>
+      </c>
+      <c r="AC9" s="10">
+        <v>382.39</v>
+      </c>
+      <c r="AD9" s="10">
+        <v>63.731666666666662</v>
+      </c>
+      <c r="AE9"/>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
+      <c r="AK9"/>
+      <c r="AL9"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>`94510A240 &lt;https://www.mcmaster.com/#94510A240&gt;`_</v>
+        <v>`3505-0804-3216 &lt;https://www.gobilda.com/3505-series-lead-screw-pattern-nut-8mm-lead-4-start-32mm-od-16mm-length/&gt;`_</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>18</v>
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
       </c>
       <c r="G10" s="6">
-        <v>7.2</v>
+        <v>8.99</v>
       </c>
       <c r="H10" s="1">
-        <v>50</v>
-      </c>
-      <c r="I10" s="7">
-        <f>A10*BOM!$L$2</f>
-        <v>180</v>
-      </c>
-      <c r="J10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="17">
         <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" si="3"/>
+        <v>8.99</v>
+      </c>
+      <c r="L10" s="17">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M10" s="17">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N10" s="6">
+        <f t="shared" si="6"/>
+        <v>8.99</v>
+      </c>
+      <c r="O10" s="17">
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="K10" s="1">
-        <f>J10*G10/BOM!$L$2</f>
-        <v>2.88</v>
-      </c>
-      <c r="L10" s="13">
+      <c r="P10" s="17">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="Q10" s="6">
+        <f t="shared" si="9"/>
+        <v>8.99</v>
+      </c>
+      <c r="R10" s="17">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="S10" s="17">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="T10" s="6">
+        <f t="shared" si="12"/>
+        <v>8.99</v>
+      </c>
+      <c r="U10" s="17">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="V10" s="17">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="W10" s="6">
+        <f t="shared" si="15"/>
+        <v>8.99</v>
+      </c>
+      <c r="X10" s="17">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="Y10" s="17">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="Z10" s="6">
+        <f t="shared" si="18"/>
+        <v>8.99</v>
+      </c>
+      <c r="AB10" s="11">
         <v>7</v>
       </c>
-      <c r="M10" s="11">
-        <v>685.3900000000001</v>
-      </c>
-      <c r="N10" s="11">
-        <v>114.23166666666668</v>
-      </c>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
-      <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10"/>
+      <c r="AC10" s="10">
+        <v>456.25</v>
+      </c>
+      <c r="AD10" s="10">
+        <v>65.178571428571431</v>
+      </c>
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
+      <c r="AK10"/>
+      <c r="AL10"/>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>`9657K267 &lt;https://www.mcmaster.com/#9657K267&gt;`_</v>
+        <v>`1612-0815-0045 &lt;https://www.gobilda.com/1612-series-linear-ball-bearing-8mm-id-x-15mm-od-45mm-length-2-pack/&gt;`_</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="6">
-        <v>10.51</v>
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="1">
+        <v>7.99</v>
       </c>
       <c r="H11" s="1">
+        <v>2</v>
+      </c>
+      <c r="I11" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J11" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" si="3"/>
+        <v>7.99</v>
+      </c>
+      <c r="L11" s="17">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M11" s="17">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N11" s="6">
+        <f t="shared" si="6"/>
+        <v>3.9950000000000001</v>
+      </c>
+      <c r="O11" s="17">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="P11" s="17">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="Q11" s="6">
+        <f t="shared" si="9"/>
+        <v>3.9950000000000001</v>
+      </c>
+      <c r="R11" s="17">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="S11" s="17">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="T11" s="6">
+        <f t="shared" si="12"/>
+        <v>3.9949999999999997</v>
+      </c>
+      <c r="U11" s="17">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="V11" s="17">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="W11" s="6">
+        <f t="shared" si="15"/>
+        <v>3.9950000000000001</v>
+      </c>
+      <c r="X11" s="17">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="Y11" s="17">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="Z11" s="6">
+        <f t="shared" si="18"/>
+        <v>3.9950000000000001</v>
+      </c>
+      <c r="AB11" s="11">
+        <v>8</v>
+      </c>
+      <c r="AC11" s="10">
+        <v>502.62</v>
+      </c>
+      <c r="AD11" s="10">
+        <v>62.827500000000001</v>
+      </c>
+      <c r="AE11"/>
+      <c r="AF11"/>
+      <c r="AG11"/>
+      <c r="AH11"/>
+      <c r="AI11"/>
+      <c r="AJ11"/>
+      <c r="AK11"/>
+      <c r="AL11"/>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="7">
-        <f>A11*BOM!$L$2</f>
-        <v>40</v>
-      </c>
-      <c r="J11" s="7">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="K11" s="1">
-        <f>J11*G11/BOM!$L$2</f>
-        <v>4.2039999999999997</v>
-      </c>
-      <c r="L11" s="13">
-        <v>8</v>
-      </c>
-      <c r="M11" s="11">
-        <v>902.62999999999988</v>
-      </c>
-      <c r="N11" s="11">
-        <v>112.82874999999999</v>
-      </c>
-      <c r="O11"/>
-      <c r="P11"/>
-      <c r="Q11"/>
-      <c r="R11"/>
-      <c r="S11"/>
-      <c r="T11"/>
-      <c r="U11"/>
-      <c r="V11"/>
-    </row>
-    <row r="12" spans="1:27">
-      <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>`6479K78 &lt;https://www.mcmaster.com/#6479K78&gt;`_</v>
+        <v>`2100-0008-0200 &lt;https://www.gobilda.com/2100-series-stainless-steel-round-shaft-8mm-diameter-200mm-length/&gt;`_</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="6">
+        <v>3.89</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="3"/>
+        <v>3.89</v>
+      </c>
+      <c r="L12" s="17">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M12" s="17">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" si="6"/>
+        <v>3.89</v>
+      </c>
+      <c r="O12" s="17">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="P12" s="17">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="Q12" s="6">
+        <f t="shared" si="9"/>
+        <v>3.89</v>
+      </c>
+      <c r="R12" s="17">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="S12" s="17">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="T12" s="6">
+        <f t="shared" si="12"/>
+        <v>3.89</v>
+      </c>
+      <c r="U12" s="17">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="V12" s="17">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="W12" s="6">
+        <f t="shared" si="15"/>
+        <v>3.89</v>
+      </c>
+      <c r="X12" s="17">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="Y12" s="17">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="Z12" s="6">
+        <f t="shared" si="18"/>
+        <v>3.8899999999999997</v>
+      </c>
+      <c r="AB12" s="11">
+        <v>9</v>
+      </c>
+      <c r="AC12" s="10">
+        <v>565.97</v>
+      </c>
+      <c r="AD12" s="10">
+        <v>62.885555555555555</v>
+      </c>
+      <c r="AE12"/>
+      <c r="AF12"/>
+      <c r="AG12"/>
+      <c r="AH12"/>
+      <c r="AI12"/>
+      <c r="AJ12"/>
+      <c r="AK12"/>
+      <c r="AL12"/>
+      <c r="AN12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>`B07Q5Q3DCB &lt;https://www.amazon.com/Befenybay-Coupling-Diameter-Coupler-Aluminum/dp/B07Q5Q3DCB/ref=sr_1_1?keywords=B07Q5Q3DCB&amp;qid=1565137893&amp;s=gateway&amp;sr=8-1&gt;`_</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="6">
+        <v>8.99</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
+      <c r="I13" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="3"/>
+        <v>8.99</v>
+      </c>
+      <c r="L13" s="17">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M13" s="17">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="6"/>
+        <v>4.4950000000000001</v>
+      </c>
+      <c r="O13" s="17">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="P13" s="17">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="Q13" s="6">
+        <f t="shared" si="9"/>
+        <v>4.4950000000000001</v>
+      </c>
+      <c r="R13" s="17">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="S13" s="17">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="T13" s="6">
+        <f t="shared" si="12"/>
+        <v>4.4950000000000001</v>
+      </c>
+      <c r="U13" s="17">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="V13" s="17">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="W13" s="6">
+        <f t="shared" si="15"/>
+        <v>4.4950000000000001</v>
+      </c>
+      <c r="X13" s="17">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="Y13" s="17">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="Z13" s="6">
+        <f t="shared" si="18"/>
+        <v>4.4950000000000001</v>
+      </c>
+      <c r="AB13" s="11">
+        <v>10</v>
+      </c>
+      <c r="AC13" s="13">
+        <v>622.85</v>
+      </c>
+      <c r="AD13" s="10">
+        <v>62.285000000000004</v>
+      </c>
+      <c r="AE13"/>
+      <c r="AF13"/>
+      <c r="AG13"/>
+      <c r="AH13"/>
+      <c r="AI13"/>
+      <c r="AJ13"/>
+      <c r="AK13"/>
+      <c r="AL13"/>
+      <c r="AM13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="6">
-        <v>5.33</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="I12" s="7">
-        <f>A12*BOM!$L$2</f>
+      <c r="AN13" s="1">
+        <v>86.9</v>
+      </c>
+      <c r="AO13" s="1">
+        <v>36.94</v>
+      </c>
+      <c r="AP13" s="1">
+        <v>31.56</v>
+      </c>
+      <c r="AQ13" s="1">
+        <v>30.22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>`255-5122-ND &lt;https://www.digikey.com/products/en?keywords=255-5122-nd&gt;`_</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="6">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="17">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J14" s="17">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="3"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L14" s="17">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="M14" s="17">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="6"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="O14" s="17">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="P14" s="17">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="Q14" s="6">
+        <f t="shared" si="9"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="R14" s="17">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="S14" s="17">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="T14" s="6">
+        <f t="shared" si="12"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="U14" s="17">
+        <f t="shared" si="13"/>
+        <v>16</v>
+      </c>
+      <c r="V14" s="17">
+        <f t="shared" si="14"/>
+        <v>16</v>
+      </c>
+      <c r="W14" s="6">
+        <f t="shared" si="15"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="X14" s="17">
+        <f t="shared" si="16"/>
+        <v>20</v>
+      </c>
+      <c r="Y14" s="17">
+        <f t="shared" si="17"/>
+        <v>20</v>
+      </c>
+      <c r="Z14" s="6">
+        <f t="shared" si="18"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
+      <c r="AL14"/>
+      <c r="AM14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN14" s="1">
+        <v>105.3</v>
+      </c>
+      <c r="AO14" s="1">
+        <v>49.22</v>
+      </c>
+      <c r="AP14" s="1">
+        <v>45.29</v>
+      </c>
+      <c r="AQ14" s="1">
+        <v>42.15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>`277-2296-ND &lt;https://www.digikey.com/products/en?keywords=277-2296-nd&gt;`_</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1.39</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="17">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J15" s="17">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" si="3"/>
+        <v>2.78</v>
+      </c>
+      <c r="L15" s="17">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="M15" s="17">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N15" s="6">
+        <f t="shared" si="6"/>
+        <v>2.78</v>
+      </c>
+      <c r="O15" s="17">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="P15" s="17">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="Q15" s="6">
+        <f t="shared" si="9"/>
+        <v>2.78</v>
+      </c>
+      <c r="R15" s="17">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="S15" s="17">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="T15" s="6">
+        <f t="shared" si="12"/>
+        <v>2.78</v>
+      </c>
+      <c r="U15" s="17">
+        <f t="shared" si="13"/>
+        <v>16</v>
+      </c>
+      <c r="V15" s="17">
+        <f t="shared" si="14"/>
+        <v>16</v>
+      </c>
+      <c r="W15" s="6">
+        <f t="shared" si="15"/>
+        <v>2.78</v>
+      </c>
+      <c r="X15" s="17">
+        <f t="shared" si="16"/>
+        <v>20</v>
+      </c>
+      <c r="Y15" s="17">
+        <f t="shared" si="17"/>
+        <v>20</v>
+      </c>
+      <c r="Z15" s="6">
+        <f t="shared" si="18"/>
+        <v>2.78</v>
+      </c>
+      <c r="AE15"/>
+      <c r="AF15"/>
+      <c r="AG15"/>
+      <c r="AH15"/>
+      <c r="AI15"/>
+      <c r="AJ15"/>
+      <c r="AK15"/>
+      <c r="AL15"/>
+      <c r="AM15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN15" s="9">
+        <v>110.8</v>
+      </c>
+      <c r="AO15" s="1">
+        <v>52</v>
+      </c>
+      <c r="AP15" s="1">
+        <v>48.74</v>
+      </c>
+      <c r="AQ15" s="1">
+        <v>45.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>`17HS24-0644S &lt;https://www.omc-stepperonline.com/hybrid-stepper-motor/nema-17-bipolar-18deg-60ncm-85ozin-064a-10v-42x42x60mm-4-wires-17hs24-0644s.html?search=17hs24-0644s&gt;`_</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="6">
+        <v>18.39</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J16" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="6">
+        <f t="shared" si="3"/>
+        <v>18.39</v>
+      </c>
+      <c r="L16" s="17">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M16" s="17">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N16" s="6">
+        <f t="shared" si="6"/>
+        <v>18.39</v>
+      </c>
+      <c r="O16" s="17">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="P16" s="17">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="Q16" s="6">
+        <f t="shared" si="9"/>
+        <v>18.39</v>
+      </c>
+      <c r="R16" s="17">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="S16" s="17">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="T16" s="6">
+        <f t="shared" si="12"/>
+        <v>18.39</v>
+      </c>
+      <c r="U16" s="17">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="V16" s="17">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="W16" s="6">
+        <f t="shared" si="15"/>
+        <v>18.39</v>
+      </c>
+      <c r="X16" s="17">
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
-      <c r="J12" s="7">
-        <f t="shared" si="2"/>
+      <c r="Y16" s="17">
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
-      <c r="K12" s="1">
-        <f>J12*G12/BOM!$L$2</f>
-        <v>5.33</v>
-      </c>
-      <c r="L12" s="13">
-        <v>9</v>
-      </c>
-      <c r="M12" s="11">
-        <v>1006.2399999999999</v>
-      </c>
-      <c r="N12" s="11">
-        <v>111.80444444444443</v>
-      </c>
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
-      <c r="R12"/>
-      <c r="S12"/>
-      <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12"/>
-      <c r="X12" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>50</v>
+      <c r="Z16" s="6">
+        <f t="shared" si="18"/>
+        <v>18.39</v>
+      </c>
+      <c r="AE16"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
+      <c r="AI16"/>
+      <c r="AJ16"/>
+      <c r="AK16"/>
+      <c r="AL16"/>
+      <c r="AM16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN16" s="1">
+        <v>152.4</v>
+      </c>
+      <c r="AO16" s="1">
+        <v>45.04</v>
+      </c>
+      <c r="AP16" s="1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="AQ16" s="1">
+        <v>28.51</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
-      <c r="A13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="2" t="s">
+    <row r="17" spans="11:38" x14ac:dyDescent="0.2">
+      <c r="K17" s="10">
+        <f>ROUNDUP(SUM(K2:K16),0)</f>
+        <v>112</v>
+      </c>
+      <c r="N17" s="10">
+        <f>ROUNDUP(SUM(N2:N16),0)</f>
+        <v>84</v>
+      </c>
+      <c r="Q17" s="10">
+        <f>ROUNDUP(SUM(Q2:Q16),0)</f>
+        <v>78</v>
+      </c>
+      <c r="T17" s="10">
+        <f>ROUNDUP(SUM(T2:T16),0)</f>
+        <v>74</v>
+      </c>
+      <c r="W17" s="10">
+        <f>ROUNDUP(SUM(W2:W16),0)</f>
+        <v>73</v>
+      </c>
+      <c r="Z17" s="10">
+        <f>ROUNDUP(SUM(Z2:Z16),0)</f>
         <v>72</v>
       </c>
-      <c r="C13" s="1" t="str">
-        <f t="shared" ref="C13:C19" si="4">CONCATENATE("`",E13," &lt;",F13,"&gt;`_")</f>
-        <v>`3501-0804-0350 &lt;https://www.servocity.com/lead-screws#371=448&gt;`_</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="6">
-        <v>7.99</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
-      <c r="I13" s="7">
-        <f>A13*BOM!$L$2</f>
-        <v>10</v>
-      </c>
-      <c r="J13" s="7">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="K13" s="1">
-        <f>J13*G13/BOM!$L$2</f>
-        <v>7.99</v>
-      </c>
-      <c r="L13" s="13">
-        <v>10</v>
-      </c>
-      <c r="M13" s="15">
-        <v>1107.97</v>
-      </c>
-      <c r="N13" s="11">
-        <v>110.797</v>
-      </c>
-      <c r="O13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
-      <c r="R13"/>
-      <c r="S13"/>
-      <c r="T13"/>
-      <c r="U13"/>
-      <c r="V13"/>
-      <c r="W13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X13" s="1">
-        <v>86.9</v>
-      </c>
-      <c r="Y13" s="1">
-        <v>36.94</v>
-      </c>
-      <c r="Z13" s="1">
-        <v>31.56</v>
-      </c>
-      <c r="AA13" s="1">
-        <v>30.22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27">
-      <c r="A14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>`545315 &lt;https://www.servocity.com/8mm-4-start-hub&gt;`_</v>
-      </c>
-      <c r="E14" s="1">
-        <v>545315</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="6">
-        <v>7.99</v>
-      </c>
-      <c r="H14" s="1">
-        <v>1</v>
-      </c>
-      <c r="I14" s="7">
-        <f>A14*BOM!$L$2</f>
-        <v>10</v>
-      </c>
-      <c r="J14" s="7">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="K14" s="1">
-        <f>J14*G14/BOM!$L$2</f>
-        <v>7.99</v>
-      </c>
-      <c r="O14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
-      <c r="R14"/>
-      <c r="S14"/>
-      <c r="T14"/>
-      <c r="U14"/>
-      <c r="V14"/>
-      <c r="W14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="X14" s="1">
-        <v>105.3</v>
-      </c>
-      <c r="Y14" s="1">
-        <v>49.22</v>
-      </c>
-      <c r="Z14" s="1">
-        <v>45.29</v>
-      </c>
-      <c r="AA14" s="1">
-        <v>42.15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27">
-      <c r="A15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>`634310 &lt;https://www.servocity.com/8mm-stainless-steel-precision-shafting#371=460&gt;`_</v>
-      </c>
-      <c r="E15" s="1">
-        <v>634310</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="6">
-        <v>3.49</v>
-      </c>
-      <c r="H15" s="1">
-        <v>1</v>
-      </c>
-      <c r="I15" s="7">
-        <f>A15*BOM!$L$2</f>
-        <v>10</v>
-      </c>
-      <c r="J15" s="7">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="K15" s="1">
-        <f>J15*G15/BOM!$L$2</f>
-        <v>3.4900000000000007</v>
-      </c>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-      <c r="R15"/>
-      <c r="S15"/>
-      <c r="T15"/>
-      <c r="U15"/>
-      <c r="V15"/>
-      <c r="W15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="X15" s="10">
-        <v>110.8</v>
-      </c>
-      <c r="Y15" s="1">
-        <v>52</v>
-      </c>
-      <c r="Z15" s="1">
-        <v>48.74</v>
-      </c>
-      <c r="AA15" s="1">
-        <v>45.56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27">
-      <c r="A16" s="3">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>`B07Q5Q3DCB &lt;https://www.amazon.com/Befenybay-Coupling-Diameter-Coupler-Aluminum/dp/B07Q5Q3DCB/ref=sr_1_1?keywords=B07Q5Q3DCB&amp;qid=1565137893&amp;s=gateway&amp;sr=8-1&gt;`_</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="6">
-        <v>8.99</v>
-      </c>
-      <c r="H16" s="1">
-        <v>2</v>
-      </c>
-      <c r="I16" s="7">
-        <f>A16*BOM!$L$2</f>
-        <v>10</v>
-      </c>
-      <c r="J16" s="7">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="K16" s="1">
-        <f>J16*G16/BOM!$L$2</f>
-        <v>4.4950000000000001</v>
-      </c>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-      <c r="R16"/>
-      <c r="S16"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="X16" s="1">
-        <v>152.4</v>
-      </c>
-      <c r="Y16" s="1">
-        <v>45.04</v>
-      </c>
-      <c r="Z16" s="1">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="AA16" s="1">
-        <v>28.51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22">
-      <c r="A17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>`B00NQ2H8YUF17 &lt;https://www.amazon.com/s?k=LMF8UU&amp;ref=nb_sb_noss_2&gt;`_</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="6">
-        <v>7.11</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-      <c r="I17" s="7">
-        <v>1</v>
-      </c>
-      <c r="J17" s="7">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K17" s="1">
-        <f>J17*G17/BOM!$L$2</f>
-        <v>0.71100000000000008</v>
-      </c>
-      <c r="L17" s="14"/>
-      <c r="N17" s="11">
-        <f>N4-N13</f>
-        <v>68.803000000000026</v>
-      </c>
-      <c r="O17"/>
-      <c r="P17"/>
-      <c r="Q17"/>
-      <c r="R17"/>
-      <c r="S17"/>
-      <c r="T17"/>
-      <c r="U17"/>
-      <c r="V17"/>
-    </row>
-    <row r="18" spans="1:22">
-      <c r="A18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>`255-5122-ND &lt;https://www.digikey.com/products/en?keywords=255-5122-nd&gt;`_</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="6">
-        <v>5.05</v>
-      </c>
-      <c r="H18" s="1">
-        <v>144</v>
-      </c>
-      <c r="I18" s="7">
-        <f>A18*BOM!$L$2</f>
-        <v>20</v>
-      </c>
-      <c r="J18" s="7">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K18" s="1">
-        <f>J18*G18/BOM!$L$2</f>
-        <v>0.505</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
-      <c r="A19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>`277-2296-ND &lt;https://www.digikey.com/products/en?keywords=277-2296-nd&gt;`_</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" s="6">
-        <v>1.39</v>
-      </c>
-      <c r="H19" s="1">
-        <v>1</v>
-      </c>
-      <c r="I19" s="7">
-        <f>A19*BOM!$L$2</f>
-        <v>20</v>
-      </c>
-      <c r="J19" s="7">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="K19" s="1">
-        <f>J19*G19/BOM!$L$2</f>
-        <v>2.78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22">
-      <c r="A20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="1" t="str">
-        <f>CONCATENATE("`",E20," &lt;",F20,"&gt;`_")</f>
-        <v>`17HS24-0644S &lt;https://www.omc-stepperonline.com/hybrid-stepper-motor/nema-17-bipolar-18deg-60ncm-85ozin-064a-10v-42x42x60mm-4-wires-17hs24-0644s.html?search=17hs24-0644s&gt;`_</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="6">
-        <v>18.39</v>
-      </c>
-      <c r="H20" s="1">
-        <v>1</v>
-      </c>
-      <c r="I20" s="7">
-        <f>A20*BOM!$L$2</f>
-        <v>10</v>
-      </c>
-      <c r="J20" s="7">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="K20" s="1">
-        <f>J20*G20/BOM!$L$2</f>
-        <v>18.39</v>
-      </c>
+      <c r="AB17" s="12"/>
+      <c r="AD17" s="10">
+        <f>AD4-AD13</f>
+        <v>43.784999999999989</v>
+      </c>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AI17"/>
+      <c r="AJ17"/>
+      <c r="AK17"/>
+      <c r="AL17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="A13:A15 A16" numberStoredAsText="1"/>
-  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -3812,7 +4681,7 @@
       <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>